<commit_message>
Auto stash before merge of "ADDAdevelopment" and "origin/ADDAdevelopment"
Updates :)
</commit_message>
<xml_diff>
--- a/ADDA/Linux/CorrectionFactors.xlsx
+++ b/ADDA/Linux/CorrectionFactors.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>dpl</t>
   </si>
@@ -55,6 +55,18 @@
   </si>
   <si>
     <t>Final Results for Polystyrene Bead in water (Radius 1 micro m)</t>
+  </si>
+  <si>
+    <t>Polystyrene cone in water (Radius 1, Height 2 micro m)</t>
+  </si>
+  <si>
+    <t>Final Results for Polystyrene cone in water (Radius 1, Height 2 micro m)</t>
+  </si>
+  <si>
+    <t>Just considering F_z</t>
+  </si>
+  <si>
+    <t>Considering F_x,F_y,F_z</t>
   </si>
 </sst>
 </file>
@@ -381,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,6 +431,9 @@
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -504,6 +519,9 @@
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -522,7 +540,7 @@
         <v>0.117050056</v>
       </c>
       <c r="G11" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -538,6 +556,9 @@
       <c r="D12">
         <v>2</v>
       </c>
+      <c r="G12" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -551,6 +572,26 @@
       </c>
       <c r="D13">
         <v>2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>1.0640000000000001</v>
+      </c>
+      <c r="C15">
+        <v>1.1859519223999999</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="G15" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to the GiT including recent runs of Brownian Motion and Beam focus variations
</commit_message>
<xml_diff>
--- a/ADDA/Linux/CorrectionFactors.xlsx
+++ b/ADDA/Linux/CorrectionFactors.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>dpl</t>
   </si>
@@ -67,6 +67,15 @@
   </si>
   <si>
     <t>Considering F_x,F_y,F_z</t>
+  </si>
+  <si>
+    <t>Propellor</t>
+  </si>
+  <si>
+    <t>Polystyrene propellor in water (Width 2, Height 2 micro m)</t>
+  </si>
+  <si>
+    <t>Final Results for Polystyrene propellor in water (Width 2, Height 2 micro m)</t>
   </si>
 </sst>
 </file>
@@ -393,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,7 +478,7 @@
         <v>2</v>
       </c>
       <c r="E4">
-        <v>0.30831057330799999</v>
+        <v>0.308310574</v>
       </c>
       <c r="G4" t="s">
         <v>5</v>
@@ -537,7 +546,7 @@
         <v>2</v>
       </c>
       <c r="E11">
-        <v>0.117050056</v>
+        <v>0.11705164730000001</v>
       </c>
       <c r="G11" t="s">
         <v>12</v>
@@ -555,6 +564,9 @@
       </c>
       <c r="D12">
         <v>2</v>
+      </c>
+      <c r="E12">
+        <v>0.31412896309999999</v>
       </c>
       <c r="G12" t="s">
         <v>5</v>
@@ -590,8 +602,87 @@
       <c r="D15">
         <v>2</v>
       </c>
+      <c r="E15">
+        <v>0.1324294717</v>
+      </c>
       <c r="G15" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>0.9</v>
+      </c>
+      <c r="C19">
+        <v>1.1859519223999999</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="G19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>15</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1.5</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="G20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>30</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>1.5</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="G21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>15</v>
+      </c>
+      <c r="B23">
+        <v>1.0640000000000001</v>
+      </c>
+      <c r="C23">
+        <v>1.1859519223999999</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="G23" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Varying Gaussian data for Spheres, Cones and Propellor
</commit_message>
<xml_diff>
--- a/ADDA/Linux/CorrectionFactors.xlsx
+++ b/ADDA/Linux/CorrectionFactors.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -405,7 +405,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,7 +512,8 @@
         <v>1.0640000000000001</v>
       </c>
       <c r="C7">
-        <v>1.1859519223999999</v>
+        <f>((((1.4435*(B7*B7))/((B7*B7)-0.020216))+1)^0.5)/1.328</f>
+        <v>1.1833903469627773</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -597,7 +598,8 @@
         <v>1.0640000000000001</v>
       </c>
       <c r="C15">
-        <v>1.1859519223999999</v>
+        <f>((((1.4435*(B15*B15))/((B15*B15)-0.020216))+1)^0.5)/1.328</f>
+        <v>1.1833903469627773</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -682,7 +684,8 @@
         <v>1.0640000000000001</v>
       </c>
       <c r="C23">
-        <v>1.1859519223999999</v>
+        <f>((((1.4435*(B23*B23))/((B23*B23)-0.020216))+1)^0.5)/1.328</f>
+        <v>1.1833903469627773</v>
       </c>
       <c r="D23">
         <v>2</v>

</xml_diff>

<commit_message>
Quick update including the start of hte twin beam arrangement
</commit_message>
<xml_diff>
--- a/ADDA/Linux/CorrectionFactors.xlsx
+++ b/ADDA/Linux/CorrectionFactors.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>dpl</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>Final Results for Polystyrene propellor in water (Width 2, Height 2 micro m)</t>
+  </si>
+  <si>
+    <t>Custom Sphere</t>
+  </si>
+  <si>
+    <t>Final Results for custom Polystyrene Bead in water (Radius 1 micro m)</t>
   </si>
 </sst>
 </file>
@@ -402,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,6 +703,35 @@
         <v>18</v>
       </c>
     </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>15</v>
+      </c>
+      <c r="B26">
+        <v>1.0640000000000001</v>
+      </c>
+      <c r="C26">
+        <f>((((1.4435*(B26*B26))/((B26*B26)-0.020216))+1)^0.5)/1.328</f>
+        <v>1.1833903469627773</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+      <c r="E26">
+        <v>8.9647142400000004E-2</v>
+      </c>
+      <c r="G26" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Dynamics updated to output Micrometres
</commit_message>
<xml_diff>
--- a/ADDA/Linux/CorrectionFactors.xlsx
+++ b/ADDA/Linux/CorrectionFactors.xlsx
@@ -125,9 +125,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,6 +733,24 @@
         <v>20</v>
       </c>
     </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>20000</v>
+      </c>
+      <c r="B27">
+        <v>1.0640000000000001</v>
+      </c>
+      <c r="C27">
+        <f>((((1.4435*(B27*B27))/((B27*B27)-0.020216))+1)^0.5)/1.328</f>
+        <v>1.1833903469627773</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27">
+        <v>8.8978163900000004E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated working yGaussian scripts and Correction Factors. Waiting for the yGaussian for Sphere and Corrected Sphere to dictate the progression of the project
</commit_message>
<xml_diff>
--- a/ADDA/Linux/CorrectionFactors.xlsx
+++ b/ADDA/Linux/CorrectionFactors.xlsx
@@ -412,7 +412,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,6 +593,9 @@
       <c r="D13">
         <v>2</v>
       </c>
+      <c r="E13">
+        <v>0.3160978559</v>
+      </c>
       <c r="G13" t="s">
         <v>6</v>
       </c>
@@ -678,6 +681,9 @@
       </c>
       <c r="D21">
         <v>2</v>
+      </c>
+      <c r="E21">
+        <v>0.14254470129999999</v>
       </c>
       <c r="G21" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Brownian verification and twin beam dynamics for size 1
</commit_message>
<xml_diff>
--- a/ADDA/Linux/CorrectionFactors.xlsx
+++ b/ADDA/Linux/CorrectionFactors.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337BFEE6-633E-4F05-93E8-E295F0447188}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>dpl</t>
   </si>
@@ -82,12 +83,15 @@
   </si>
   <si>
     <t>Final Results for custom Polystyrene Bead in water (Radius 1 micro m)</t>
+  </si>
+  <si>
+    <t>For Hopping purposes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -408,11 +412,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,32 +536,32 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1064</v>
+      </c>
+      <c r="C8" s="2">
+        <v>11851752494</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0.1836997782</v>
+      </c>
+      <c r="G8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>15</v>
-      </c>
-      <c r="B11">
-        <v>0.9</v>
-      </c>
-      <c r="C11">
-        <v>1.1859519223999999</v>
-      </c>
-      <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="E11">
-        <v>0.11705164730000001</v>
-      </c>
-      <c r="G11" t="s">
-        <v>12</v>
+      <c r="B11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -565,24 +569,24 @@
         <v>15</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="C12">
-        <v>1.5</v>
+        <v>1.1859519223999999</v>
       </c>
       <c r="D12">
         <v>2</v>
       </c>
       <c r="E12">
-        <v>0.31412896309999999</v>
+        <v>0.11705164730000001</v>
       </c>
       <c r="G12" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -594,59 +598,59 @@
         <v>2</v>
       </c>
       <c r="E13">
+        <v>0.31412896309999999</v>
+      </c>
+      <c r="G13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>30</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1.5</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
         <v>0.3160978559</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>15</v>
-      </c>
-      <c r="B15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
         <v>1.0640000000000001</v>
       </c>
-      <c r="C15">
-        <f>((((1.4435*(B15*B15))/((B15*B15)-0.020216))+1)^0.5)/1.328</f>
+      <c r="C16">
+        <f>((((1.4435*(B16*B16))/((B16*B16)-0.020216))+1)^0.5)/1.328</f>
         <v>1.1833903469627773</v>
       </c>
-      <c r="D15">
-        <v>2</v>
-      </c>
-      <c r="E15">
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
         <v>0.1324294717</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>15</v>
-      </c>
-      <c r="B19">
-        <v>0.9</v>
-      </c>
-      <c r="C19">
-        <v>1.1859519223999999</v>
-      </c>
-      <c r="D19">
-        <v>2</v>
-      </c>
-      <c r="E19">
-        <v>9.3815007800000003E-2</v>
-      </c>
-      <c r="G19" t="s">
-        <v>17</v>
+      <c r="B19" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -654,24 +658,24 @@
         <v>15</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="C20">
-        <v>1.5</v>
+        <v>1.1859519223999999</v>
       </c>
       <c r="D20">
         <v>2</v>
       </c>
       <c r="E20">
-        <v>0.14571586480000001</v>
+        <v>9.3815007800000003E-2</v>
       </c>
       <c r="G20" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -683,65 +687,64 @@
         <v>2</v>
       </c>
       <c r="E21">
+        <v>0.14571586480000001</v>
+      </c>
+      <c r="G21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>30</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1.5</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
         <v>0.14254470129999999</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G22" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>15</v>
-      </c>
-      <c r="B23">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>15</v>
+      </c>
+      <c r="B24">
         <v>1.0640000000000001</v>
       </c>
-      <c r="C23">
-        <f>((((1.4435*(B23*B23))/((B23*B23)-0.020216))+1)^0.5)/1.328</f>
+      <c r="C24">
+        <f>((((1.4435*(B24*B24))/((B24*B24)-0.020216))+1)^0.5)/1.328</f>
         <v>1.1833903469627773</v>
       </c>
-      <c r="D23">
-        <v>2</v>
-      </c>
-      <c r="E23">
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24">
         <v>0.10964010120000001</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G24" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>15</v>
-      </c>
-      <c r="B26">
-        <v>1.0640000000000001</v>
-      </c>
-      <c r="C26">
-        <f>((((1.4435*(B26*B26))/((B26*B26)-0.020216))+1)^0.5)/1.328</f>
-        <v>1.1833903469627773</v>
-      </c>
-      <c r="D26">
-        <v>2</v>
-      </c>
-      <c r="E26">
-        <v>8.9647142400000004E-2</v>
-      </c>
-      <c r="G26" t="s">
-        <v>20</v>
-      </c>
-    </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <v>20000</v>
+      <c r="A27">
+        <v>15</v>
       </c>
       <c r="B27">
         <v>1.0640000000000001</v>
@@ -754,6 +757,27 @@
         <v>2</v>
       </c>
       <c r="E27">
+        <v>8.9647142400000004E-2</v>
+      </c>
+      <c r="G27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>20000</v>
+      </c>
+      <c r="B28">
+        <v>1.0640000000000001</v>
+      </c>
+      <c r="C28">
+        <f>((((1.4435*(B28*B28))/((B28*B28)-0.020216))+1)^0.5)/1.328</f>
+        <v>1.1833903469627773</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28">
         <v>8.8978163900000004E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Initial counterpropagating beam dynamics
</commit_message>
<xml_diff>
--- a/ADDA/Linux/CorrectionFactors.xlsx
+++ b/ADDA/Linux/CorrectionFactors.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337BFEE6-633E-4F05-93E8-E295F0447188}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A860C6-025D-41AC-8DB8-DA4BBED88E00}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -416,7 +416,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,7 +544,7 @@
         <v>1064</v>
       </c>
       <c r="C8" s="2">
-        <v>11851752494</v>
+        <v>1.1851752494000001</v>
       </c>
       <c r="D8">
         <v>1</v>

</xml_diff>